<commit_message>
Made reference cells mandatory to simplify the reading of the files, changes to test data and documentation as necessary.  Also added stub of converter routine.
</commit_message>
<xml_diff>
--- a/tests/data/empty_row.xlsx
+++ b/tests/data/empty_row.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>station</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>lon</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>UNAM</t>
   </si>
 </sst>
 </file>
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,86 +542,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
       <c r="J2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>20.043185999999999</v>
-      </c>
-      <c r="E3" s="1">
-        <v>-100.71677699999999</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.72367753123320733</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
       <c r="J3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>16.874293999999999</v>
+        <v>20.043185999999999</v>
       </c>
       <c r="E4" s="1">
-        <v>-99.886505</v>
+        <v>-100.71677699999999</v>
       </c>
       <c r="F4" s="4">
-        <v>4.0075548582081897</v>
+        <v>0.72367753123320733</v>
       </c>
       <c r="J4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -624,52 +617,52 @@
         <v>5</v>
       </c>
       <c r="D5" s="1">
-        <v>17.213360999999999</v>
+        <v>16.874293999999999</v>
       </c>
       <c r="E5" s="1">
-        <v>-100.43226900000001</v>
+        <v>-99.886505</v>
       </c>
       <c r="F5" s="4">
-        <v>2.9940900430465254</v>
+        <v>4.0075548582081897</v>
       </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1">
-        <v>16.247374000000001</v>
+        <v>17.213360999999999</v>
       </c>
       <c r="E6" s="1">
-        <v>-93.912575000000004</v>
+        <v>-100.43226900000001</v>
       </c>
       <c r="F6" s="4">
-        <v>0</v>
+        <v>2.9940900430465254</v>
       </c>
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1">
-        <v>19.325265999999999</v>
+        <v>16.247374000000001</v>
       </c>
       <c r="E7" s="1">
-        <v>-103.760813</v>
+        <v>-93.912575000000004</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -678,28 +671,28 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1">
-        <v>16.997788</v>
+        <v>19.325265999999999</v>
       </c>
       <c r="E8" s="1">
-        <v>-100.089963</v>
+        <v>-103.760813</v>
       </c>
       <c r="F8" s="4">
-        <v>2.9623072177545042</v>
+        <v>0</v>
       </c>
       <c r="J8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
@@ -708,40 +701,40 @@
         <v>5</v>
       </c>
       <c r="D9" s="1">
-        <v>17.798341000000001</v>
+        <v>16.997788</v>
       </c>
       <c r="E9" s="1">
-        <v>-98.559717000000006</v>
+        <v>-100.089963</v>
       </c>
       <c r="F9" s="4">
-        <v>6.5085773089009038</v>
+        <v>2.9623072177545042</v>
       </c>
       <c r="J9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="1">
-        <v>16.565152999999999</v>
+        <v>17.798341000000001</v>
       </c>
       <c r="E10" s="1">
-        <v>-94.616946999999996</v>
+        <v>-98.559717000000006</v>
       </c>
       <c r="F10" s="4">
-        <v>1.1827263333975842</v>
+        <v>6.5085773089009038</v>
       </c>
       <c r="J10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
@@ -750,19 +743,19 @@
         <v>5</v>
       </c>
       <c r="D11" s="1">
-        <v>17.067336999999998</v>
+        <v>16.565152999999999</v>
       </c>
       <c r="E11" s="1">
-        <v>-96.723804000000001</v>
+        <v>-94.616946999999996</v>
       </c>
       <c r="F11" s="4">
-        <v>2.9439815281494539</v>
+        <v>1.1827263333975842</v>
       </c>
       <c r="J11"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
@@ -771,19 +764,19 @@
         <v>5</v>
       </c>
       <c r="D12" s="1">
-        <v>17.065038999999999</v>
+        <v>17.067336999999998</v>
       </c>
       <c r="E12" s="1">
-        <v>-96.703157000000004</v>
+        <v>-96.723804000000001</v>
       </c>
       <c r="F12" s="4">
-        <v>3.2904002934162691</v>
+        <v>2.9439815281494539</v>
       </c>
       <c r="J12"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -792,170 +785,191 @@
         <v>5</v>
       </c>
       <c r="D13" s="1">
-        <v>15.666836999999999</v>
+        <v>17.065038999999999</v>
       </c>
       <c r="E13" s="1">
-        <v>-96.490505999999996</v>
+        <v>-96.703157000000004</v>
       </c>
       <c r="F13" s="4">
-        <v>0.79309982225129416</v>
+        <v>3.2904002934162691</v>
       </c>
       <c r="J13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="1">
-        <v>17.535395999999999</v>
+        <v>15.666836999999999</v>
       </c>
       <c r="E14" s="1">
-        <v>-101.262608</v>
+        <v>-96.490505999999996</v>
       </c>
       <c r="F14" s="4">
-        <v>2.0047614148547304</v>
+        <v>0.79309982225129416</v>
       </c>
       <c r="J14"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="1">
-        <v>19.044222999999999</v>
+        <v>17.535395999999999</v>
       </c>
       <c r="E15" s="1">
-        <v>-98.168465999999995</v>
+        <v>-101.262608</v>
       </c>
       <c r="F15" s="4">
-        <v>6.2143501408750526</v>
+        <v>2.0047614148547304</v>
       </c>
       <c r="J15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1">
-        <v>18.904050999999999</v>
+        <v>19.044222999999999</v>
       </c>
       <c r="E16" s="1">
-        <v>-100.159615</v>
+        <v>-98.168465999999995</v>
       </c>
       <c r="F16" s="4">
-        <v>5.3695607051488423</v>
+        <v>6.2143501408750526</v>
       </c>
       <c r="J16"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="1">
-        <v>17.98762</v>
+        <v>18.904050999999999</v>
       </c>
       <c r="E17" s="1">
-        <v>-101.81062300000001</v>
+        <v>-100.159615</v>
       </c>
       <c r="F17" s="4">
-        <v>1.2090871001382097</v>
+        <v>5.3695607051488423</v>
       </c>
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="1">
-        <v>19.421758000000001</v>
+        <v>17.98762</v>
       </c>
       <c r="E18" s="1">
-        <v>-102.07405900000001</v>
+        <v>-101.81062300000001</v>
       </c>
       <c r="F18" s="4">
-        <v>1.1985951953533427</v>
+        <v>1.2090871001382097</v>
       </c>
       <c r="J18"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="1">
-        <v>16.914259999999999</v>
+        <v>19.421758000000001</v>
       </c>
       <c r="E19" s="1">
-        <v>-99.818849999999998</v>
+        <v>-102.07405900000001</v>
       </c>
       <c r="F19" s="4">
-        <v>2.0971117481552666</v>
+        <v>1.1985951953533427</v>
       </c>
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1">
+        <v>16.914259999999999</v>
+      </c>
+      <c r="E20" s="1">
+        <v>-99.818849999999998</v>
+      </c>
+      <c r="F20" s="4">
+        <v>2.0971117481552666</v>
+      </c>
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="C21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1">
         <v>19.529875000000001</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E21" s="1">
         <v>-96.901972999999998</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F21" s="4">
         <v>1.6999910326326615</v>
       </c>
-      <c r="J20"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F21" s="6"/>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F22" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1" tooltip="Michoacán" display="https://en.wikipedia.org/wiki/Michoac%C3%A1n"/>
-    <hyperlink ref="B20" r:id="rId2" tooltip="Veracruz" display="https://en.wikipedia.org/wiki/Veracruz"/>
+    <hyperlink ref="B19" r:id="rId1" tooltip="Michoacán" display="https://en.wikipedia.org/wiki/Michoac%C3%A1n"/>
+    <hyperlink ref="B21" r:id="rId2" tooltip="Veracruz" display="https://en.wikipedia.org/wiki/Veracruz"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>